<commit_message>
Refactor backend and improve ESP32 RFID integration
Refactored server.js for better structure, robust Excel handling, and improved API responses. Enhanced ESP32 test code with clearer registration/access logic, improved web UI, and more reliable backend communication. Updated users.xlsx to reflect new user data format.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -111,13 +111,13 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <family val="2"/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <family val="2"/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -184,6 +184,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -494,7 +500,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -589,58 +595,74 @@
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D9" s="2">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add UID-to-username lookup and login hint feature
Introduced a new /uid-name/:uid endpoint in the server for direct UID-to-username lookup. Updated the ESP32 test code to fetch and suggest usernames for login based on scanned RFID cards, including a new /login-hint route and frontend auto-fill logic. Updated users.xlsx with new data.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>user</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>F9B351E9</t>
   </si>
 </sst>
 </file>
@@ -500,7 +506,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -545,7 +551,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="6">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>9</v>
@@ -657,12 +663,32 @@
         <v>20</v>
       </c>
       <c r="D9" s="2">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add auto-refresh to status page HTML output
Introduced a JavaScript snippet to auto-refresh the status page every 2 seconds for real-time updates. Also adjusted HTML structure and duplicated last stats JSON display logic for improved visibility.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>user</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>F9B351E9</t>
+  </si>
+  <si>
+    <t>poooq</t>
+  </si>
+  <si>
+    <t>E9956AF6</t>
   </si>
 </sst>
 </file>
@@ -506,7 +512,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -551,7 +557,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>9</v>
@@ -663,7 +669,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>21</v>
@@ -683,12 +689,32 @@
         <v>24</v>
       </c>
       <c r="D10" s="2">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update users.xlsx with latest user data
The users.xlsx file has been updated to reflect recent changes in user information. This may include additions, removals, or modifications to user records.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
   <si>
     <t>user</t>
   </si>
@@ -49,90 +49,46 @@
     <t>true</t>
   </si>
   <si>
-    <t>charlie</t>
-  </si>
-  <si>
-    <t>pass3</t>
-  </si>
-  <si>
-    <t>19AF56E9</t>
-  </si>
-  <si>
-    <t>103|202</t>
-  </si>
-  <si>
-    <t>Jacobe</t>
-  </si>
-  <si>
-    <t>pass4</t>
-  </si>
-  <si>
-    <t>202|204</t>
-  </si>
-  <si>
     <t/>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>EA4C7814</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>F9B351E9</t>
-  </si>
-  <si>
-    <t>poooq</t>
-  </si>
-  <si>
-    <t>E9956AF6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -148,7 +104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -171,54 +127,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="15">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -512,210 +484,178 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.147857142857141" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.147857142857141" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.147857142857141" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.147857142857141" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.719285714285713" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.147857142857141" style="1" customWidth="1"/>
+    <col min="1" max="1" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6">
-        <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="5">
+        <v>25</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="6">
-        <v>6</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="6">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2">
-        <v>21</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2">
-        <v>30</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="2">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>22</v>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve RFID event handling and access feedback
Refactored handleCardUid to clarify delete, registration, and access modes. Enhanced access denial feedback for 404 responses and added suppression of repeated 'No new card' messages in the main loop. Updated users.xlsx with new user data.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>user</t>
   </si>
@@ -34,38 +34,23 @@
     <t>access</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>E9956AF6</t>
+    <t>YAHYA</t>
+  </si>
+  <si>
+    <t>EA4C7814</t>
   </si>
   <si>
     <t>101</t>
   </si>
   <si>
     <t>TRUE</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>EA4C7814</t>
-  </si>
-  <si>
-    <t>YAHYA</t>
-  </si>
-  <si>
-    <t>591EF2D4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -84,19 +69,13 @@
       <color rgb="FF000000"/>
       <family val="2"/>
       <sz val="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <family val="2"/>
-      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <color rgb="FF000000"/>
       <family val="2"/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -108,7 +87,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFf2f2f2"/>
       </patternFill>
     </fill>
   </fills>
@@ -122,16 +101,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -139,14 +118,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -157,21 +139,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -196,10 +172,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -237,71 +213,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -329,7 +305,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -352,11 +328,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -365,13 +341,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -381,7 +357,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -390,7 +366,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -399,7 +375,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -407,10 +383,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -479,192 +455,178 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.45" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.73046875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.147857142857141" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.147857142857141" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.147857142857141" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.147857142857141" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.719285714285713" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.147857142857141" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" ht="19.5" customHeight="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+    <row r="2" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" ht="20.25" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2">
-        <v>4</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enable dynamic room selection via potentiometer
Added potentiometer support to ESP32 access control to allow dynamic room selection. Updated server registration logic to append new rooms to existing UIDs and improved feedback messages. Adjusted potentiometer test code for room number mapping and increased serial baud rate.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>user</t>
   </si>
@@ -34,16 +34,22 @@
     <t>access</t>
   </si>
   <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>EA4C7814</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
     <t>YAHYA</t>
   </si>
   <si>
-    <t>EA4C7814</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>TRUE</t>
+    <t>110</t>
   </si>
 </sst>
 </file>
@@ -455,7 +461,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -610,22 +616,50 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="2">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add minimal RFID reader example and improve throttling
Added Minimal_reader.ino as a simple RFID reader test sketch. Improved message and log throttling in esp32_access_control_full.ino to reduce serial spam. Updated users.xlsx with new data.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>user</t>
   </si>
@@ -34,22 +34,19 @@
     <t>access</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>EA4C7814</t>
-  </si>
-  <si>
-    <t>100</t>
+    <t>YAHYA</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>591EF2D4</t>
+  </si>
+  <si>
+    <t>103|100</t>
   </si>
   <si>
     <t>TRUE</t>
-  </si>
-  <si>
-    <t>YAHYA</t>
-  </si>
-  <si>
-    <t>110</t>
   </si>
 </sst>
 </file>
@@ -461,7 +458,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -624,43 +621,55 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="2">
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2">
         <v>0</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add RGB LED support and update hardware logic
Introduced RGB LED control via PWM in esp32_access_control_full.ino, refactored indicator logic to use color feedback, and updated hardware pin assignments. Changed WiFi credentials and backend URLs for local network. Added SMD_RGB.ino test sketch for RGB LED, updated circuit image, and modified users.xlsx data.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>user</t>
   </si>
@@ -37,13 +37,10 @@
     <t>YAHYA</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>591EF2D4</t>
-  </si>
-  <si>
-    <t>103|100</t>
+    <t>EA4C7814</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
   <si>
     <t>TRUE</t>
@@ -458,7 +455,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -653,23 +650,55 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D26" s="2">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add room deletion feature to access control system
Implemented room-specific deletion via touch sensor and card scan in esp32_access_control_full.ino, including new logic for arming room delete mode and handling room removal. Added /room/:uid/:roomID DELETE endpoint to server.js for safe room removal from users, updating users.xlsx accordingly. Updated Display_On_Screen.ino to a simple I2C scanner for hardware debugging.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>user</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>EA4C7814</t>
+  </si>
+  <si>
+    <t>105|103</t>
   </si>
 </sst>
 </file>
@@ -455,7 +461,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -709,6 +715,66 @@
         <v>9</v>
       </c>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add request logging to logs.xlsx and update server
Introduces a new logs.xlsx file and implements request logging for all HTTP routes in server.js. Each request is logged with details such as timestamp, protocol, method, route, status, result, user, UID, roomID, message, and IP. Logging middleware and log initialization are added, and all major routes now include contextual log messages. Also updates users.xlsx with new data.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -46,17 +46,17 @@
     <t>TRUE</t>
   </si>
   <si>
-    <t>EA4C7814</t>
-  </si>
-  <si>
-    <t>105|103</t>
+    <t>6BF02F00</t>
+  </si>
+  <si>
+    <t>103</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -72,16 +72,10 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <family val="2"/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-      <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -124,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -146,15 +140,6 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,7 +446,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -496,282 +481,42 @@
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" ht="20.25" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" ht="20.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="2">
-        <v>5</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="2">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix access normalization and update user counter logic
Improved access normalization by trimming whitespace before converting to lowercase. Replaced the previous counter update logic with a new function that increments the user's counter directly in the Excel file and updates the in-memory value, ensuring consistency between the database and application state.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -46,10 +46,10 @@
     <t>TRUE</t>
   </si>
   <si>
+    <t>TEST</t>
+  </si>
+  <si>
     <t>6BF02F00</t>
-  </si>
-  <si>
-    <t>103</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -501,22 +501,30 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="D4" s="2">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve code formatting and web UI for ESP32 access control
Refactored code for better readability and consistency across .ino files, including expanded enum formatting and improved comments. Enhanced the web UI status page with color-coded indicators, collapsible JSON display, and additional system information for better diagnostics. Updated Excel files for logs and users.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>user</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>105|104|103|101</t>
+  </si>
+  <si>
+    <t>frrr</t>
+  </si>
+  <si>
+    <t>EA4C7814</t>
+  </si>
+  <si>
+    <t>103</t>
   </si>
 </sst>
 </file>
@@ -449,7 +458,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -579,6 +588,50 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="2">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add buzzer patterns and dashboard auto-refresh
Introduced distinct buzzer feedback patterns for various access control events in hardware_ui.ino, improving user interaction and status indication. Enhanced dashboard.ejs with client-side auto-refresh for users and logs tables, supported by a new /admin/data endpoint in website.js for live data updates.

----
still motor dosent work ;(
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>user</t>
   </si>
@@ -46,22 +46,10 @@
     <t>TRUE</t>
   </si>
   <si>
-    <t>TEST</t>
+    <t>gggd</t>
   </si>
   <si>
     <t>6BF02F00</t>
-  </si>
-  <si>
-    <t>105|104|103|101</t>
-  </si>
-  <si>
-    <t>frrr</t>
-  </si>
-  <si>
-    <t>EA4C7814</t>
-  </si>
-  <si>
-    <t>103</t>
   </si>
 </sst>
 </file>
@@ -458,7 +446,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -521,24 +509,12 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2">
-        <v>45</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -613,22 +589,38 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor door control to use servo instead of relay
Replaces relay-based door lock logic with servo motor control in the ESP32 access control example. Updates hardware UI and main logic to support non-blocking servo movement, adds servo configuration and helpers, and introduces a test sketch for periodic servo operation. Also updates pin assignments and removes relay references.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/users.xlsx
+++ b/Server/rfid-server-DBS-Http/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>user</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>6BF02F00</t>
+  </si>
+  <si>
+    <t>frrr</t>
+  </si>
+  <si>
+    <t>EA4C7814</t>
+  </si>
+  <si>
+    <t>106</t>
   </si>
 </sst>
 </file>
@@ -446,7 +455,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -491,7 +500,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>8</v>
@@ -615,12 +624,32 @@
         <v>11</v>
       </c>
       <c r="D16" s="2">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>